<commit_message>
add acceleration to state and integrate
</commit_message>
<xml_diff>
--- a/data/WLTC.xlsx
+++ b/data/WLTC.xlsx
@@ -5648,11 +5648,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="10399289"/>
-        <c:axId val="76141792"/>
+        <c:axId val="66752186"/>
+        <c:axId val="81542525"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="10399289"/>
+        <c:axId val="66752186"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5680,12 +5680,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76141792"/>
+        <c:crossAx val="81542525"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76141792"/>
+        <c:axId val="81542525"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5722,7 +5722,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10399289"/>
+        <c:crossAx val="66752186"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5775,15 +5775,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>36720</xdr:colOff>
+      <xdr:colOff>37080</xdr:colOff>
       <xdr:row>245</xdr:row>
       <xdr:rowOff>122400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>195120</xdr:colOff>
+      <xdr:colOff>194400</xdr:colOff>
       <xdr:row>272</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5791,8 +5791,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2411280" y="43061040"/>
-        <a:ext cx="8505720" cy="4784400"/>
+        <a:off x="2411640" y="43061040"/>
+        <a:ext cx="8504640" cy="4784040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5813,10 +5813,10 @@
   <dimension ref="A1:C1802"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="F181" activeCellId="0" sqref="F181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.83"/>

</xml_diff>